<commit_message>
Field Defined and Configure
- Field Definition MovieScreen [home] Screen Code : MOVIE0101
- Configure Screen Code [Update]
</commit_message>
<xml_diff>
--- a/document/Design/Configuration.xlsx
+++ b/document/Design/Configuration.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Tello Tag Configuration" sheetId="1" r:id="rId1"/>
+    <sheet name="Tello Tag and Screen Code Conf." sheetId="1" r:id="rId1"/>
     <sheet name="Resource" sheetId="3" r:id="rId2"/>
-    <sheet name="Version Control Configuration" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tello Tag Configuration'!$A$2:$G$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tello Tag and Screen Code Conf.'!$A$2:$H$28</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="106">
   <si>
     <t>Trello Tag Configuration</t>
   </si>
@@ -35,9 +34,6 @@
     <t>Tag Type</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Tag Code</t>
   </si>
   <si>
@@ -77,9 +73,6 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>Movie - List</t>
-  </si>
-  <si>
     <t>Account</t>
   </si>
   <si>
@@ -89,9 +82,6 @@
     <t>Search Account</t>
   </si>
   <si>
-    <t>Movie - Management</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -185,12 +175,6 @@
     <t>Cyan</t>
   </si>
   <si>
-    <t>ACLOG0101</t>
-  </si>
-  <si>
-    <t>Sign In Screen</t>
-  </si>
-  <si>
     <t>Review</t>
   </si>
   <si>
@@ -200,24 +184,6 @@
     <t>Review Card Complete</t>
   </si>
   <si>
-    <t>Version Pattern</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Maintenance Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deploy Project </t>
-  </si>
-  <si>
-    <t>ACLOG0102</t>
-  </si>
-  <si>
     <t>Forgot Password</t>
   </si>
   <si>
@@ -233,66 +199,159 @@
     <t>MOVIE0201</t>
   </si>
   <si>
-    <t>Movie - Detail</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>add</t>
-  </si>
-  <si>
     <t>Bootstrap 3</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
-    <t>Jython</t>
-  </si>
-  <si>
-    <t>Springframework</t>
-  </si>
-  <si>
     <t>Tools</t>
   </si>
   <si>
-    <t>Eclipse EE Luna</t>
-  </si>
-  <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>Maven</t>
-  </si>
-  <si>
-    <t>Lib +++++++</t>
-  </si>
-  <si>
-    <t>AngularJS 1.5</t>
-  </si>
-  <si>
-    <t>Workbench 6.3 CE</t>
-  </si>
-  <si>
-    <t>HeidiSQL 7</t>
-  </si>
-  <si>
-    <t>Tomcat 7</t>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
+    <t>Description (EN)</t>
+  </si>
+  <si>
+    <t>Description (TH)</t>
+  </si>
+  <si>
+    <t>เอกสารสำหรับดำเนินการโครงงาน</t>
+  </si>
+  <si>
+    <t>เอกสารสำหรับนำเสนอ</t>
+  </si>
+  <si>
+    <t>เอกสารสำหรับอาจารย์ที่ปรึกษา</t>
+  </si>
+  <si>
+    <t>การออกแบบระบบ</t>
+  </si>
+  <si>
+    <t>หน้าจอสำหรับแสดงผลการใช้งาน</t>
+  </si>
+  <si>
+    <t>หน้าแรก</t>
+  </si>
+  <si>
+    <t>ภาพยนต์ทั้งหมด</t>
+  </si>
+  <si>
+    <t>คนชอบมากที่สุด</t>
+  </si>
+  <si>
+    <t>ติดต่อเรา</t>
+  </si>
+  <si>
+    <t>Public Favorite</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>backlog</t>
+  </si>
+  <si>
+    <t>MOVIE0103</t>
+  </si>
+  <si>
+    <t>MOVIE0301</t>
+  </si>
+  <si>
+    <t>จัดการภาพยนต์</t>
+  </si>
+  <si>
+    <t>Movies Management</t>
+  </si>
+  <si>
+    <t>ค้นหาบัญชีผู้ใช้</t>
+  </si>
+  <si>
+    <t>จัดการบัญชีผู้ใช้</t>
+  </si>
+  <si>
+    <t>เข้าสู่ระบบ</t>
+  </si>
+  <si>
+    <t>ลืมรหัสผ่าน</t>
+  </si>
+  <si>
+    <t>สมัครสมาชิก</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>HTML5</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Flask</t>
+  </si>
+  <si>
+    <t>VueJs</t>
+  </si>
+  <si>
+    <t>Jquery</t>
+  </si>
+  <si>
+    <t>Axios</t>
+  </si>
+  <si>
+    <t>Cors</t>
+  </si>
+  <si>
+    <t>Framework and Library</t>
+  </si>
+  <si>
+    <t>Pandas and Numpy</t>
+  </si>
+  <si>
+    <t>Sparse</t>
+  </si>
+  <si>
+    <t>Scipy</t>
+  </si>
+  <si>
+    <t>Eclipse Luna</t>
+  </si>
+  <si>
+    <t>PyDev</t>
+  </si>
+  <si>
+    <t>GitHub Subversion Control</t>
+  </si>
+  <si>
+    <t>MOVIE0104</t>
+  </si>
+  <si>
+    <t>ภาพยนต์ทั้งหมด แบ่งตามหมวดหมู่</t>
+  </si>
+  <si>
+    <t>[Genres] Movies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -300,12 +359,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,8 +383,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -419,26 +484,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -476,34 +526,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,23 +820,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.625" customWidth="1"/>
-    <col min="2" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="30.625" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -808,8 +846,9 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -817,644 +856,823 @@
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>6</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>21</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="C24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="H25" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>19</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="21" t="s">
+      <c r="B26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C26" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>24</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="C27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="H27" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>25</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>22</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="G28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G24" xr:uid="{FA0238DB-8F8F-4C9A-8203-5D4B17E6088E}"/>
+  <autoFilter ref="A2:H28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFC4931-1D01-4AD9-8F7C-8B9EB784D162}">
-  <dimension ref="A2:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="18" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" t="s">
-        <v>85</v>
+    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68935A50-2479-48AD-B4FF-4F0F09EC5E00}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="5" width="14.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>